<commit_message>
4 hours study sessions changed to Envio Catequistas: Sunday, 19 Feb
</commit_message>
<xml_diff>
--- a/Calendario 4 Semanas.xlsx
+++ b/Calendario 4 Semanas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateo Arango Valenci\OneDrive - Universidad de Antioquia\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateo Arango Valenci\OneDrive - Universidad de Antioquia\Documentos\repositorio prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D628390-2918-476E-A998-5DFB7629D6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1FAF59-3975-4336-9CC8-8868D7A005CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B998CF33-F9ED-401C-92F1-2C42874B65F6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="32">
   <si>
     <t>L</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Semana 5-11 MARZO</t>
+  </si>
+  <si>
+    <t>Envio Catequistas</t>
   </si>
 </sst>
 </file>
@@ -501,7 +504,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,7 +819,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -842,7 +845,7 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -1374,6 +1377,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006704263559FC6548BD288283575EDAD8" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="4110cb85e99cbe5a24c723887aff7754">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="847f3826-a425-43aa-a10e-248d9a81c14c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3d8a9e488af22a953af62f3abd7e689a" ns3:_="">
     <xsd:import namespace="847f3826-a425-43aa-a10e-248d9a81c14c"/>
@@ -1563,15 +1575,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1579,6 +1582,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7D87DD-15B9-41AA-AF44-F62716654036}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97ED4328-41DA-4A5B-96D4-D62B15BEDEF0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1592,14 +1603,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7D87DD-15B9-41AA-AF44-F62716654036}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>